<commit_message>
Asia to Europe for Turkey, Brasil to Chile for PUC Santiago
</commit_message>
<xml_diff>
--- a/geodiverse_data.xlsx
+++ b/geodiverse_data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{800DB39A-5FA5-8448-AAE0-57CD75418887}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514005F7-D4EB-42B9-BE6A-1C763B139906}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35880" windowHeight="15220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -16499,29 +16503,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N2369"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="H1854" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M1872" sqref="M1872"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="43.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5" customWidth="1"/>
-    <col min="3" max="3" width="16.1640625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="43.46484375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.46484375" customWidth="1"/>
+    <col min="3" max="3" width="16.1328125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="21.46484375" customWidth="1"/>
     <col min="5" max="5" width="17.6640625" customWidth="1"/>
     <col min="6" max="6" width="24.33203125" customWidth="1"/>
     <col min="7" max="7" width="74.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5" customWidth="1"/>
+    <col min="8" max="8" width="12.46484375" customWidth="1"/>
     <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.796875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="49.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5" customWidth="1"/>
+    <col min="12" max="12" width="11.46484375" customWidth="1"/>
     <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="24.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1" ht="16" thickBot="1">
+    <row r="1" spans="1:14" s="2" customFormat="1" ht="14.65" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -64331,7 +64335,7 @@
         <v>4556</v>
       </c>
     </row>
-    <row r="1486" spans="1:10" ht="16">
+    <row r="1486" spans="1:10">
       <c r="A1486" t="s">
         <v>2338</v>
       </c>
@@ -64555,7 +64559,7 @@
         <v>5114</v>
       </c>
     </row>
-    <row r="1493" spans="1:10" ht="16">
+    <row r="1493" spans="1:10">
       <c r="A1493" t="s">
         <v>2338</v>
       </c>
@@ -64587,7 +64591,7 @@
         <v>4902</v>
       </c>
     </row>
-    <row r="1494" spans="1:10" ht="16">
+    <row r="1494" spans="1:10">
       <c r="A1494" t="s">
         <v>2338</v>
       </c>
@@ -64651,7 +64655,7 @@
         <v>3589</v>
       </c>
     </row>
-    <row r="1496" spans="1:10" ht="16">
+    <row r="1496" spans="1:10">
       <c r="A1496" t="s">
         <v>2338</v>
       </c>
@@ -64683,7 +64687,7 @@
         <v>4383</v>
       </c>
     </row>
-    <row r="1497" spans="1:10" ht="16">
+    <row r="1497" spans="1:10">
       <c r="A1497" t="s">
         <v>2338</v>
       </c>
@@ -64779,7 +64783,7 @@
         <v>4292</v>
       </c>
     </row>
-    <row r="1500" spans="1:10" ht="16">
+    <row r="1500" spans="1:10">
       <c r="A1500" t="s">
         <v>2338</v>
       </c>
@@ -65186,7 +65190,7 @@
         <v>3074</v>
       </c>
       <c r="H1512" t="s">
-        <v>2993</v>
+        <v>2938</v>
       </c>
       <c r="I1512" s="6" t="s">
         <v>3149</v>
@@ -76769,7 +76773,7 @@
         <v>2953</v>
       </c>
       <c r="M1872" t="s">
-        <v>3152</v>
+        <v>3151</v>
       </c>
       <c r="N1872" s="11" t="s">
         <v>5335</v>
@@ -92601,7 +92605,7 @@
       <c r="C2369" s="3"/>
     </row>
   </sheetData>
-  <sortState ref="A2:N2369">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N2369">
     <sortCondition ref="A2:A2369"/>
     <sortCondition ref="D2:D2369"/>
     <sortCondition ref="F2:F2369"/>
@@ -92619,17 +92623,17 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="56.6640625" customWidth="1"/>
-    <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="12.46484375" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5" customWidth="1"/>
+    <col min="6" max="6" width="15.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16" thickBot="1">
+    <row r="1" spans="1:6" ht="14.65" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>5344</v>
       </c>
@@ -101781,7 +101785,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:C419" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
-  <sortState ref="A2:F419">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F419">
     <sortCondition descending="1" ref="E2:E419"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -101796,14 +101800,14 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.1328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" thickBot="1">
+    <row r="1" spans="1:4" ht="14.65" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>2909</v>
       </c>
@@ -102130,7 +102134,7 @@
       </c>
       <c r="C21" s="6">
         <f>COUNTIF(Data!H:H,A21)+COUNTIF(Data!L:L,A21)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D21">
         <f>COUNTIFS(Data!H:H,A21,Data!B:B,"1")+COUNTIFS(Data!L:L,A21,Data!B:B,"1")</f>
@@ -102290,7 +102294,7 @@
       </c>
       <c r="C31" s="6">
         <f>COUNTIF(Data!H:H,A31)+COUNTIF(Data!L:L,A31)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D31">
         <f>COUNTIFS(Data!H:H,A31,Data!B:B,"1")+COUNTIFS(Data!L:L,A31,Data!B:B,"1")</f>
@@ -102523,7 +102527,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:B45" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
-  <sortState ref="A2:D45">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D45">
     <sortCondition descending="1" ref="C2:C45"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -102538,12 +102542,12 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="3" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" thickBot="1">
+    <row r="1" spans="1:3" ht="14.65" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>3147</v>
       </c>
@@ -102573,7 +102577,7 @@
       </c>
       <c r="B3" s="6">
         <f>COUNTIF(Data!I:I,A3)+COUNTIF(Data!M:M,A3)</f>
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="C3">
         <f>COUNTIFS(Data!I:I,A3,Data!B:B,"1")+COUNTIFS(Data!M:M,A3,Data!B:B,"1")</f>
@@ -102599,7 +102603,7 @@
       </c>
       <c r="B5" s="6">
         <f>COUNTIF(Data!I:I,A5)+COUNTIF(Data!M:M,A5)</f>
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C5">
         <f>COUNTIFS(Data!I:I,A5,Data!B:B,"1")+COUNTIFS(Data!M:M,A5,Data!B:B,"1")</f>
@@ -102646,7 +102650,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:B426">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B426">
     <sortCondition descending="1" ref="B2:B426"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Columbia to Colombia for country
</commit_message>
<xml_diff>
--- a/geodiverse_data.xlsx
+++ b/geodiverse_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514005F7-D4EB-42B9-BE6A-1C763B139906}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61D079F0-7ED6-49F7-825E-998733E69ED1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20825" uniqueCount="5358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20825" uniqueCount="5359">
   <si>
     <t>Journal</t>
   </si>
@@ -16110,6 +16110,9 @@
   </si>
   <si>
     <t>is_Top5</t>
+  </si>
+  <si>
+    <t>Colombia</t>
   </si>
 </sst>
 </file>
@@ -16503,8 +16506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N2369"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1854" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M1872" sqref="M1872"/>
+    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
@@ -35844,7 +35847,7 @@
         <v>925</v>
       </c>
       <c r="H598" s="6" t="s">
-        <v>212</v>
+        <v>5358</v>
       </c>
       <c r="I598" s="6" t="s">
         <v>3149</v>
@@ -102406,7 +102409,7 @@
       </c>
       <c r="C38" s="6">
         <f>COUNTIF(Data!H:H,A38)+COUNTIF(Data!L:L,A38)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D38">
         <f>COUNTIFS(Data!H:H,A38,Data!B:B,"1")+COUNTIFS(Data!L:L,A38,Data!B:B,"1")</f>

</xml_diff>